<commit_message>
Deleted old number cleaning
</commit_message>
<xml_diff>
--- a/Usage/Partner_Kalender_Duos.xlsx
+++ b/Usage/Partner_Kalender_Duos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CVR\App\Usage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4D8A34-0DAC-4F3D-A515-07F6B00A5AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2949378C-C729-4FE3-AFB3-EA149900F07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Alle ERA Partner</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Claas Seefeld</t>
+  </si>
+  <si>
+    <t>Stephan Morbitzer</t>
+  </si>
+  <si>
+    <t>Zahide Jashari (Optional Morbitzer)</t>
   </si>
 </sst>
 </file>
@@ -577,19 +583,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,13 +603,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -611,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -619,7 +625,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -627,19 +633,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -647,7 +653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -655,13 +661,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -669,31 +675,31 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -701,13 +707,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -715,7 +721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -723,79 +729,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -803,7 +809,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -811,13 +817,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
@@ -825,25 +831,25 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -851,30 +857,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="5"/>
     </row>
-    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="5"/>
     </row>
-    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>50</v>
       </c>
       <c r="B42" s="5"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
       <c r="B43" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>